<commit_message>
updates on ccordinates 05072021
</commit_message>
<xml_diff>
--- a/data/TablesZhangetal2017_WV.xlsx
+++ b/data/TablesZhangetal2017_WV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E7A1CE-5782-497F-B08A-AC4E4A16CA91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6963F5-A3CB-49DC-B8E5-659BB61DA4E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12624" activeTab="1" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
   </bookViews>
   <sheets>
     <sheet name="Zhang et al. (2017) &gt;1000km2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="609">
   <si>
     <t>Watershed #</t>
   </si>
@@ -1825,9 +1825,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Approximate location using original report (Schneider &amp; Ayer 1961) and google maps</t>
-  </si>
-  <si>
     <t>willem</t>
   </si>
   <si>
@@ -1882,13 +1879,37 @@
     <t>duplicates of Troendle and King?</t>
   </si>
   <si>
-    <t>not in the Hibbert reference? Seems a straight copy from Bosch and Hewlett? Why was "South Fork" not added? Coordinates from google maps</t>
-  </si>
-  <si>
-    <t>duplicate of 260?</t>
-  </si>
-  <si>
-    <t>duplicate? Not in Hibbert 1979</t>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>duplicate of 260, one single year according to Bosch and Hewlett (1982) Not in Hibbert 1979</t>
+  </si>
+  <si>
+    <t>these values are extracted from Hibbert and Gottfried (1987) but are summarised in the "Study area" section of the paper, suggested to be for 1967 - 1979 (13 years). This is for the "South Fork" part. This is repeated in the Stednick paper and is 62 in Bosch and Hewlett (1982). original publication is actually Rich and Gottfried (1976)</t>
+  </si>
+  <si>
+    <t>Related to 260 In the Stednick 1996 paper (Table 1), this result appears also Table 1 in Bosch and Hewlett (1982) and averaging the 5 years post harvesting for "North Fork" "moist site" watershed #60, but it is also in Hibbert and Gottfried (1987), who cite Rich and Gottfried (1976) for the original data, In Hibbert and Gottfried, the time period is 1959 - 1966 (7 years)</t>
+  </si>
+  <si>
+    <t>Related to 260. Again in the "Study Area" of Hibbert and Gottfried (1987) but in this case for the "North Fork" dry site. Also in the Stednick 1996 paper (Table 1), and appears in Table 1 in Bosch and Hewlett (1982) "North Fork" watershed #60 but referring to the 1% riparian vegetation cut</t>
+  </si>
+  <si>
+    <t>related to 260. The results seem to differ between Rich and Gottfried (1976) and Hibbert and Gottfried. This result is Hibbert and Gottfried (1987). The result also appears in Stednick (1996). This is the "dry site" for North Fork. Time period based on Hibbert and Gottfried (1987).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Another related to 260, Straight from Stednick 1996 paper as this result does not appear in Hibbert and Gottfried (1987) unless it is an interpretation of the storm flow). Seems to refer to North Fork dry site as in Bosch and Hewlett (1982) where they mention "residual burned (total 73% cleared). </t>
+  </si>
+  <si>
+    <t>not in the Hibbert reference. However, this seems to come from Bosch and Hewlett (1982) and either is a single year response or a duplicate of 304.</t>
+  </si>
+  <si>
+    <t>Data from https://waterdata.usgs.gov/</t>
+  </si>
+  <si>
+    <t>Original report is actually Schneider &amp; Ayer (1961) location from https://waterdata.usgs.gov/</t>
+  </si>
+  <si>
+    <t>Location from https://waterdata.usgs.gov/ Not in Brown et al. (2005), but in Bosch and Hewlett (1982). Original reference is Schneider and Ayer (1961), U.S. Geol. Surv., Water-Supply Pap. 1602.</t>
   </si>
 </sst>
 </file>
@@ -2030,6 +2051,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2042,7 +2064,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2367,54 +2388,54 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
       <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
@@ -4559,68 +4580,68 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C628113C-78B0-4B5D-8B46-887DA17257C6}">
-  <dimension ref="A1:P253"/>
+  <dimension ref="A1:Q253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P162" sqref="P162"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="B231" sqref="B231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="18" t="s">
         <v>11</v>
       </c>
       <c r="L1" s="10"/>
     </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
       <c r="L2" s="10" t="s">
         <v>530</v>
       </c>
@@ -4633,11 +4654,11 @@
       <c r="O2" t="s">
         <v>551</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>62</v>
       </c>
@@ -4673,7 +4694,7 @@
       </c>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>63</v>
       </c>
@@ -4709,7 +4730,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>64</v>
       </c>
@@ -4753,7 +4774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>65</v>
       </c>
@@ -4798,7 +4819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>66</v>
       </c>
@@ -4834,7 +4855,7 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>67</v>
       </c>
@@ -4880,11 +4901,12 @@
       <c r="O8" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="4"/>
+      <c r="Q8" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>68</v>
       </c>
@@ -4920,7 +4942,7 @@
       </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>69</v>
       </c>
@@ -4956,7 +4978,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>70</v>
       </c>
@@ -4992,7 +5014,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>71</v>
       </c>
@@ -5028,7 +5050,7 @@
       </c>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>72</v>
       </c>
@@ -5063,11 +5085,11 @@
         <v>143</v>
       </c>
       <c r="L13" s="4"/>
-      <c r="P13" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q13" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>73</v>
       </c>
@@ -5103,7 +5125,7 @@
       </c>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>74</v>
       </c>
@@ -5139,7 +5161,7 @@
       </c>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>75</v>
       </c>
@@ -5175,7 +5197,7 @@
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>76</v>
       </c>
@@ -5211,7 +5233,7 @@
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>77</v>
       </c>
@@ -5246,11 +5268,11 @@
         <v>153</v>
       </c>
       <c r="L18" s="4"/>
-      <c r="P18" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="51" x14ac:dyDescent="0.3">
+      <c r="Q18" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="51" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>78</v>
       </c>
@@ -5286,7 +5308,7 @@
       </c>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:16" ht="51" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="51" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>79</v>
       </c>
@@ -5322,7 +5344,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>80</v>
       </c>
@@ -5358,7 +5380,7 @@
       </c>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>81</v>
       </c>
@@ -5394,7 +5416,7 @@
       </c>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>82</v>
       </c>
@@ -5430,7 +5452,7 @@
       </c>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>83</v>
       </c>
@@ -5465,11 +5487,11 @@
         <v>143</v>
       </c>
       <c r="L24" s="4"/>
-      <c r="P24" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q24" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>84</v>
       </c>
@@ -5505,7 +5527,7 @@
       </c>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>85</v>
       </c>
@@ -5551,11 +5573,11 @@
       <c r="O26">
         <v>1</v>
       </c>
-      <c r="P26" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q26" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>86</v>
       </c>
@@ -5591,7 +5613,7 @@
       </c>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>87</v>
       </c>
@@ -5627,7 +5649,7 @@
       </c>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>88</v>
       </c>
@@ -5663,7 +5685,7 @@
       </c>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>89</v>
       </c>
@@ -5699,7 +5721,7 @@
       </c>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>90</v>
       </c>
@@ -5735,7 +5757,7 @@
       </c>
       <c r="L31" s="11"/>
     </row>
-    <row r="32" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>91</v>
       </c>
@@ -5771,7 +5793,7 @@
       </c>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>92</v>
       </c>
@@ -5807,7 +5829,7 @@
       </c>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>93</v>
       </c>
@@ -5843,7 +5865,7 @@
       </c>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>94</v>
       </c>
@@ -5879,7 +5901,7 @@
       </c>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>95</v>
       </c>
@@ -5914,8 +5936,22 @@
         <v>183</v>
       </c>
       <c r="L36" s="4"/>
-    </row>
-    <row r="37" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <f>42+31/60+52/3600</f>
+        <v>42.531111111111109</v>
+      </c>
+      <c r="N36">
+        <f>-(75+25/60+31/3600)</f>
+        <v>-75.425277777777779</v>
+      </c>
+      <c r="O36">
+        <v>26</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>96</v>
       </c>
@@ -5951,7 +5987,7 @@
       </c>
       <c r="L37" s="4"/>
     </row>
-    <row r="38" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>97</v>
       </c>
@@ -5987,7 +6023,7 @@
       </c>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>98</v>
       </c>
@@ -6023,7 +6059,7 @@
       </c>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>99</v>
       </c>
@@ -6059,7 +6095,7 @@
       </c>
       <c r="L40" s="4"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>100</v>
       </c>
@@ -6095,10 +6131,10 @@
       </c>
       <c r="L41" s="4"/>
       <c r="O41" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>101</v>
       </c>
@@ -6134,7 +6170,7 @@
       </c>
       <c r="L42" s="4"/>
     </row>
-    <row r="43" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>102</v>
       </c>
@@ -6169,16 +6205,18 @@
         <v>153</v>
       </c>
       <c r="M43" s="4">
-        <v>42.173830140236902</v>
+        <f>42+9/60+40/3600</f>
+        <v>42.161111111111111</v>
       </c>
       <c r="N43">
-        <v>-75.409262268186097</v>
-      </c>
-      <c r="P43" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+        <f>-75-23/60-34/3600</f>
+        <v>-75.392777777777781</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>103</v>
       </c>
@@ -6214,7 +6252,7 @@
       </c>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>104</v>
       </c>
@@ -6250,7 +6288,7 @@
       </c>
       <c r="L45" s="4"/>
     </row>
-    <row r="46" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>105</v>
       </c>
@@ -6286,7 +6324,7 @@
       </c>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>106</v>
       </c>
@@ -6322,7 +6360,7 @@
       </c>
       <c r="L47" s="4"/>
     </row>
-    <row r="48" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>107</v>
       </c>
@@ -6934,7 +6972,7 @@
       </c>
       <c r="L64" s="4"/>
     </row>
-    <row r="65" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>124</v>
       </c>
@@ -6970,7 +7008,7 @@
       </c>
       <c r="L65" s="4"/>
     </row>
-    <row r="66" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>125</v>
       </c>
@@ -7006,7 +7044,7 @@
       </c>
       <c r="L66" s="4"/>
     </row>
-    <row r="67" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>126</v>
       </c>
@@ -7051,7 +7089,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>127</v>
       </c>
@@ -7087,7 +7125,7 @@
       </c>
       <c r="L68" s="4"/>
     </row>
-    <row r="69" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>128</v>
       </c>
@@ -7123,7 +7161,7 @@
       </c>
       <c r="L69" s="4"/>
     </row>
-    <row r="70" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>129</v>
       </c>
@@ -7159,7 +7197,7 @@
       </c>
       <c r="L70" s="4"/>
     </row>
-    <row r="71" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>130</v>
       </c>
@@ -7195,7 +7233,7 @@
       </c>
       <c r="L71" s="4"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>131</v>
       </c>
@@ -7241,11 +7279,11 @@
       <c r="O72">
         <v>24</v>
       </c>
-      <c r="P72" t="s">
+      <c r="Q72" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>132</v>
       </c>
@@ -7281,7 +7319,7 @@
       </c>
       <c r="L73" s="4"/>
     </row>
-    <row r="74" spans="1:16" ht="51" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" ht="51" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>133</v>
       </c>
@@ -7317,7 +7355,7 @@
       </c>
       <c r="L74" s="4"/>
     </row>
-    <row r="75" spans="1:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>134</v>
       </c>
@@ -7353,7 +7391,7 @@
       </c>
       <c r="L75" s="4"/>
     </row>
-    <row r="76" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>135</v>
       </c>
@@ -7389,7 +7427,7 @@
       </c>
       <c r="L76" s="4"/>
     </row>
-    <row r="77" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>136</v>
       </c>
@@ -7425,7 +7463,7 @@
       </c>
       <c r="L77" s="4"/>
     </row>
-    <row r="78" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>137</v>
       </c>
@@ -7461,7 +7499,7 @@
       </c>
       <c r="L78" s="4"/>
     </row>
-    <row r="79" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>138</v>
       </c>
@@ -7497,7 +7535,7 @@
       </c>
       <c r="L79" s="4"/>
     </row>
-    <row r="80" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>139</v>
       </c>
@@ -7533,7 +7571,7 @@
       </c>
       <c r="L80" s="4"/>
     </row>
-    <row r="81" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>140</v>
       </c>
@@ -7569,7 +7607,7 @@
       </c>
       <c r="L81" s="4"/>
     </row>
-    <row r="82" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>141</v>
       </c>
@@ -7605,7 +7643,7 @@
       </c>
       <c r="L82" s="4"/>
     </row>
-    <row r="83" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>142</v>
       </c>
@@ -7641,7 +7679,7 @@
       </c>
       <c r="L83" s="4"/>
     </row>
-    <row r="84" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>143</v>
       </c>
@@ -7677,7 +7715,7 @@
       </c>
       <c r="L84" s="4"/>
     </row>
-    <row r="85" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="6">
         <v>144</v>
       </c>
@@ -7713,7 +7751,7 @@
       </c>
       <c r="L85" s="11"/>
     </row>
-    <row r="86" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>145</v>
       </c>
@@ -7749,7 +7787,7 @@
       </c>
       <c r="L86" s="4"/>
     </row>
-    <row r="87" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>146</v>
       </c>
@@ -7785,7 +7823,7 @@
       </c>
       <c r="L87" s="4"/>
     </row>
-    <row r="88" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>147</v>
       </c>
@@ -7821,7 +7859,7 @@
       </c>
       <c r="L88" s="4"/>
     </row>
-    <row r="89" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>148</v>
       </c>
@@ -7857,7 +7895,7 @@
       </c>
       <c r="L89" s="4"/>
     </row>
-    <row r="90" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>149</v>
       </c>
@@ -7893,7 +7931,7 @@
       </c>
       <c r="L90" s="4"/>
     </row>
-    <row r="91" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>150</v>
       </c>
@@ -7929,7 +7967,7 @@
       </c>
       <c r="L91" s="4"/>
     </row>
-    <row r="92" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>151</v>
       </c>
@@ -7973,11 +8011,11 @@
       <c r="O92">
         <v>30</v>
       </c>
-      <c r="P92" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q92" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>152</v>
       </c>
@@ -8021,11 +8059,11 @@
       <c r="O93">
         <v>30</v>
       </c>
-      <c r="P93" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q93" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>153</v>
       </c>
@@ -8069,11 +8107,11 @@
       <c r="O94">
         <v>30</v>
       </c>
-      <c r="P94" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="95" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="Q94" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
         <v>154</v>
       </c>
@@ -8109,7 +8147,7 @@
       </c>
       <c r="L95" s="4"/>
     </row>
-    <row r="96" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>155</v>
       </c>
@@ -8145,7 +8183,7 @@
       </c>
       <c r="L96" s="4"/>
     </row>
-    <row r="97" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
         <v>156</v>
       </c>
@@ -8189,11 +8227,11 @@
       <c r="O97">
         <v>30</v>
       </c>
-      <c r="P97" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="98" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q97" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>157</v>
       </c>
@@ -8237,11 +8275,11 @@
       <c r="O98">
         <v>30</v>
       </c>
-      <c r="P98" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="Q98" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>158</v>
       </c>
@@ -8282,11 +8320,11 @@
       <c r="N99">
         <v>-105.92363805782</v>
       </c>
-      <c r="P99" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q99" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>159</v>
       </c>
@@ -8322,7 +8360,7 @@
       </c>
       <c r="L100" s="4"/>
     </row>
-    <row r="101" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
         <v>160</v>
       </c>
@@ -8358,7 +8396,7 @@
       </c>
       <c r="L101" s="4"/>
     </row>
-    <row r="102" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>161</v>
       </c>
@@ -8394,7 +8432,7 @@
       </c>
       <c r="L102" s="4"/>
     </row>
-    <row r="103" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
         <v>162</v>
       </c>
@@ -8430,7 +8468,7 @@
       </c>
       <c r="L103" s="4"/>
     </row>
-    <row r="104" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>163</v>
       </c>
@@ -8466,7 +8504,7 @@
       </c>
       <c r="L104" s="4"/>
     </row>
-    <row r="105" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
         <v>164</v>
       </c>
@@ -8502,7 +8540,7 @@
       </c>
       <c r="L105" s="4"/>
     </row>
-    <row r="106" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
         <v>165</v>
       </c>
@@ -8538,7 +8576,7 @@
       </c>
       <c r="L106" s="4"/>
     </row>
-    <row r="107" spans="1:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
         <v>166</v>
       </c>
@@ -8574,7 +8612,7 @@
       </c>
       <c r="L107" s="4"/>
     </row>
-    <row r="108" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
         <v>167</v>
       </c>
@@ -8621,7 +8659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
         <v>168</v>
       </c>
@@ -8657,7 +8695,7 @@
       </c>
       <c r="L109" s="4"/>
     </row>
-    <row r="110" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
         <v>169</v>
       </c>
@@ -8693,7 +8731,7 @@
       </c>
       <c r="L110" s="4"/>
     </row>
-    <row r="111" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
         <v>170</v>
       </c>
@@ -8729,7 +8767,7 @@
       </c>
       <c r="L111" s="4"/>
     </row>
-    <row r="112" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
         <v>171</v>
       </c>
@@ -9341,7 +9379,7 @@
       </c>
       <c r="L128" s="4"/>
     </row>
-    <row r="129" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A129" s="4">
         <v>188</v>
       </c>
@@ -9377,7 +9415,7 @@
       </c>
       <c r="L129" s="4"/>
     </row>
-    <row r="130" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A130" s="4">
         <v>189</v>
       </c>
@@ -9413,7 +9451,7 @@
       </c>
       <c r="L130" s="4"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" s="4">
         <v>190</v>
       </c>
@@ -9449,7 +9487,7 @@
       </c>
       <c r="L131" s="4"/>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" s="4">
         <v>191</v>
       </c>
@@ -9485,7 +9523,7 @@
       </c>
       <c r="L132" s="4"/>
     </row>
-    <row r="133" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A133" s="4">
         <v>192</v>
       </c>
@@ -9521,7 +9559,7 @@
       </c>
       <c r="L133" s="4"/>
     </row>
-    <row r="134" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A134" s="4">
         <v>193</v>
       </c>
@@ -9557,7 +9595,7 @@
       </c>
       <c r="L134" s="4"/>
     </row>
-    <row r="135" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A135" s="4">
         <v>194</v>
       </c>
@@ -9593,7 +9631,7 @@
       </c>
       <c r="L135" s="4"/>
     </row>
-    <row r="136" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A136" s="4">
         <v>195</v>
       </c>
@@ -9640,7 +9678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A137" s="4">
         <v>196</v>
       </c>
@@ -9676,7 +9714,7 @@
       </c>
       <c r="L137" s="4"/>
     </row>
-    <row r="138" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A138" s="4">
         <v>197</v>
       </c>
@@ -9712,7 +9750,7 @@
       </c>
       <c r="L138" s="4"/>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" s="4">
         <v>198</v>
       </c>
@@ -9748,7 +9786,7 @@
       </c>
       <c r="L139" s="4"/>
     </row>
-    <row r="140" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A140" s="4">
         <v>199</v>
       </c>
@@ -9784,7 +9822,7 @@
       </c>
       <c r="L140" s="4"/>
     </row>
-    <row r="141" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:17" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="6">
         <v>200</v>
       </c>
@@ -9820,7 +9858,7 @@
       </c>
       <c r="L141" s="11"/>
     </row>
-    <row r="142" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A142" s="4">
         <v>201</v>
       </c>
@@ -9856,7 +9894,7 @@
       </c>
       <c r="L142" s="4"/>
     </row>
-    <row r="143" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A143" s="4">
         <v>202</v>
       </c>
@@ -9900,11 +9938,11 @@
       <c r="O143">
         <v>6</v>
       </c>
-      <c r="P143" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="144" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q143" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A144" s="4">
         <v>203</v>
       </c>
@@ -10516,7 +10554,7 @@
       </c>
       <c r="L160" s="4"/>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" s="4">
         <v>220</v>
       </c>
@@ -10551,11 +10589,20 @@
         <v>385</v>
       </c>
       <c r="L161" s="4"/>
-      <c r="P161" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="162" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="M161">
+        <v>33.788912562983</v>
+      </c>
+      <c r="N161">
+        <v>-110.963855204659</v>
+      </c>
+      <c r="O161">
+        <v>1</v>
+      </c>
+      <c r="Q161" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A162" s="4">
         <v>221</v>
       </c>
@@ -10591,7 +10638,7 @@
       </c>
       <c r="L162" s="4"/>
     </row>
-    <row r="163" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A163" s="4">
         <v>222</v>
       </c>
@@ -10635,11 +10682,11 @@
       <c r="O163">
         <v>6</v>
       </c>
-      <c r="P163" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="164" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q163" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="164" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A164" s="4">
         <v>223</v>
       </c>
@@ -10683,11 +10730,11 @@
       <c r="O164">
         <v>3</v>
       </c>
-      <c r="P164" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="165" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q164" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A165" s="4">
         <v>224</v>
       </c>
@@ -10723,7 +10770,7 @@
       </c>
       <c r="L165" s="4"/>
     </row>
-    <row r="166" spans="1:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A166" s="4">
         <v>225</v>
       </c>
@@ -10759,7 +10806,7 @@
       </c>
       <c r="L166" s="4"/>
     </row>
-    <row r="167" spans="1:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A167" s="4">
         <v>226</v>
       </c>
@@ -10795,7 +10842,7 @@
       </c>
       <c r="L167" s="4"/>
     </row>
-    <row r="168" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A168" s="4">
         <v>227</v>
       </c>
@@ -10831,7 +10878,7 @@
       </c>
       <c r="L168" s="4"/>
     </row>
-    <row r="169" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:17" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A169" s="6">
         <v>228</v>
       </c>
@@ -10867,7 +10914,7 @@
       </c>
       <c r="L169" s="11"/>
     </row>
-    <row r="170" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A170" s="4">
         <v>229</v>
       </c>
@@ -10911,11 +10958,11 @@
       <c r="O170">
         <v>6</v>
       </c>
-      <c r="P170" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="171" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q170" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="171" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A171" s="4">
         <v>230</v>
       </c>
@@ -10951,7 +10998,7 @@
       </c>
       <c r="L171" s="4"/>
     </row>
-    <row r="172" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A172" s="4">
         <v>231</v>
       </c>
@@ -10987,7 +11034,7 @@
       </c>
       <c r="L172" s="4"/>
     </row>
-    <row r="173" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A173" s="4">
         <v>232</v>
       </c>
@@ -11023,7 +11070,7 @@
       </c>
       <c r="L173" s="4"/>
     </row>
-    <row r="174" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A174" s="4">
         <v>233</v>
       </c>
@@ -11059,7 +11106,7 @@
       </c>
       <c r="L174" s="4"/>
     </row>
-    <row r="175" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A175" s="4">
         <v>234</v>
       </c>
@@ -11095,7 +11142,7 @@
       </c>
       <c r="L175" s="4"/>
     </row>
-    <row r="176" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A176" s="4">
         <v>235</v>
       </c>
@@ -11131,7 +11178,7 @@
       </c>
       <c r="L176" s="4"/>
     </row>
-    <row r="177" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A177" s="4">
         <v>236</v>
       </c>
@@ -11167,7 +11214,7 @@
       </c>
       <c r="L177" s="4"/>
     </row>
-    <row r="178" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A178" s="4">
         <v>237</v>
       </c>
@@ -11203,7 +11250,7 @@
       </c>
       <c r="L178" s="4"/>
     </row>
-    <row r="179" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A179" s="4">
         <v>238</v>
       </c>
@@ -11239,7 +11286,7 @@
       </c>
       <c r="L179" s="4"/>
     </row>
-    <row r="180" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A180" s="4">
         <v>239</v>
       </c>
@@ -11275,7 +11322,7 @@
       </c>
       <c r="L180" s="4"/>
     </row>
-    <row r="181" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A181" s="4">
         <v>240</v>
       </c>
@@ -11310,11 +11357,11 @@
         <v>290</v>
       </c>
       <c r="L181" s="4"/>
-      <c r="P181" t="s">
+      <c r="Q181" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="182" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A182" s="4">
         <v>241</v>
       </c>
@@ -11350,7 +11397,7 @@
       </c>
       <c r="L182" s="4"/>
     </row>
-    <row r="183" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A183" s="4">
         <v>242</v>
       </c>
@@ -11386,7 +11433,7 @@
       </c>
       <c r="L183" s="4"/>
     </row>
-    <row r="184" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A184" s="4">
         <v>243</v>
       </c>
@@ -11422,7 +11469,7 @@
       </c>
       <c r="L184" s="4"/>
     </row>
-    <row r="185" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A185" s="4">
         <v>244</v>
       </c>
@@ -11458,7 +11505,7 @@
       </c>
       <c r="L185" s="4"/>
     </row>
-    <row r="186" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A186" s="4">
         <v>245</v>
       </c>
@@ -11494,7 +11541,7 @@
       </c>
       <c r="L186" s="4"/>
     </row>
-    <row r="187" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A187" s="4">
         <v>246</v>
       </c>
@@ -11530,7 +11577,7 @@
       </c>
       <c r="L187" s="4"/>
     </row>
-    <row r="188" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A188" s="4">
         <v>247</v>
       </c>
@@ -11566,7 +11613,7 @@
       </c>
       <c r="L188" s="4"/>
     </row>
-    <row r="189" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A189" s="4">
         <v>248</v>
       </c>
@@ -11613,7 +11660,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="190" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A190" s="4">
         <v>249</v>
       </c>
@@ -11649,7 +11696,7 @@
       </c>
       <c r="L190" s="4"/>
     </row>
-    <row r="191" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A191" s="4">
         <v>250</v>
       </c>
@@ -11685,7 +11732,7 @@
       </c>
       <c r="L191" s="4"/>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A192" s="4">
         <v>251</v>
       </c>
@@ -12297,7 +12344,7 @@
       </c>
       <c r="L208" s="4"/>
     </row>
-    <row r="209" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A209" s="4">
         <v>294</v>
       </c>
@@ -12333,7 +12380,7 @@
       </c>
       <c r="L209" s="4"/>
     </row>
-    <row r="210" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A210" s="4">
         <v>295</v>
       </c>
@@ -12369,7 +12416,7 @@
       </c>
       <c r="L210" s="4"/>
     </row>
-    <row r="211" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A211" s="4">
         <v>296</v>
       </c>
@@ -12405,7 +12452,7 @@
       </c>
       <c r="L211" s="4"/>
     </row>
-    <row r="212" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A212" s="4">
         <v>297</v>
       </c>
@@ -12441,7 +12488,7 @@
       </c>
       <c r="L212" s="4"/>
     </row>
-    <row r="213" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A213" s="4">
         <v>298</v>
       </c>
@@ -12487,11 +12534,12 @@
       <c r="O213" s="4">
         <v>24</v>
       </c>
-      <c r="P213" t="s">
+      <c r="P213" s="4"/>
+      <c r="Q213" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A214" s="4">
         <v>299</v>
       </c>
@@ -12527,7 +12575,7 @@
       </c>
       <c r="L214" s="4"/>
     </row>
-    <row r="215" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A215" s="4">
         <v>300</v>
       </c>
@@ -12563,7 +12611,7 @@
       </c>
       <c r="L215" s="4"/>
     </row>
-    <row r="216" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A216" s="4">
         <v>301</v>
       </c>
@@ -12599,7 +12647,7 @@
       </c>
       <c r="L216" s="4"/>
     </row>
-    <row r="217" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A217" s="4">
         <v>302</v>
       </c>
@@ -12634,11 +12682,23 @@
         <v>503</v>
       </c>
       <c r="L217" s="4"/>
+      <c r="M217">
+        <v>33.788912562983</v>
+      </c>
+      <c r="N217">
+        <v>-110.963855204659</v>
+      </c>
+      <c r="O217">
+        <v>5</v>
+      </c>
       <c r="P217" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="218" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q217" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="218" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A218" s="4">
         <v>303</v>
       </c>
@@ -12673,11 +12733,20 @@
         <v>515</v>
       </c>
       <c r="L218" s="4"/>
+      <c r="M218">
+        <v>33.788912562983</v>
+      </c>
+      <c r="N218">
+        <v>-110.963855204659</v>
+      </c>
       <c r="P218" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="219" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q218" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="219" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A219" s="4">
         <v>304</v>
       </c>
@@ -12712,11 +12781,23 @@
         <v>517</v>
       </c>
       <c r="L219" s="4"/>
+      <c r="M219">
+        <v>33.788912562983</v>
+      </c>
+      <c r="N219">
+        <v>-110.963855204659</v>
+      </c>
+      <c r="O219">
+        <v>11</v>
+      </c>
       <c r="P219" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="220" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q219" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="220" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A220" s="4">
         <v>305</v>
       </c>
@@ -12751,11 +12832,23 @@
         <v>519</v>
       </c>
       <c r="L220" s="4"/>
+      <c r="M220">
+        <v>33.788912562983</v>
+      </c>
+      <c r="N220">
+        <v>-110.963855204659</v>
+      </c>
+      <c r="O220">
+        <v>13</v>
+      </c>
       <c r="P220" t="s">
+        <v>598</v>
+      </c>
+      <c r="Q220" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="221" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A221" s="4">
         <v>306</v>
       </c>
@@ -12790,11 +12883,23 @@
         <v>521</v>
       </c>
       <c r="L221" s="4"/>
+      <c r="M221">
+        <v>33.788912562983</v>
+      </c>
+      <c r="N221">
+        <v>-110.963855204659</v>
+      </c>
+      <c r="O221">
+        <v>11</v>
+      </c>
       <c r="P221" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="222" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q221" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="222" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A222" s="4">
         <v>307</v>
       </c>
@@ -12830,7 +12935,7 @@
       </c>
       <c r="L222" s="4"/>
     </row>
-    <row r="223" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A223" s="4">
         <v>308</v>
       </c>
@@ -12866,7 +12971,7 @@
       </c>
       <c r="L223" s="4"/>
     </row>
-    <row r="224" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A224" s="4">
         <v>309</v>
       </c>
@@ -12902,7 +13007,7 @@
       </c>
       <c r="L224" s="4"/>
     </row>
-    <row r="225" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A225" s="4">
         <v>310</v>
       </c>
@@ -12938,7 +13043,7 @@
       </c>
       <c r="L225" s="4"/>
     </row>
-    <row r="226" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A226" s="4">
         <v>311</v>
       </c>
@@ -12985,7 +13090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="227" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:17" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A227" s="6">
         <v>312</v>
       </c>
@@ -13020,11 +13125,11 @@
         <v>345</v>
       </c>
       <c r="L227" s="11"/>
-      <c r="P227" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="228" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q227" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="228" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A228" s="8">
         <v>257</v>
       </c>
@@ -13060,7 +13165,7 @@
       </c>
       <c r="L228" s="11"/>
     </row>
-    <row r="229" spans="1:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A229" s="4">
         <v>258</v>
       </c>
@@ -13096,7 +13201,7 @@
       </c>
       <c r="L229" s="4"/>
     </row>
-    <row r="230" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A230" s="4">
         <v>259</v>
       </c>
@@ -13131,8 +13236,22 @@
         <v>449</v>
       </c>
       <c r="L230" s="4"/>
-    </row>
-    <row r="231" spans="1:16" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="M230">
+        <f>42+46/60+2/3600</f>
+        <v>42.767222222222223</v>
+      </c>
+      <c r="N230">
+        <f>-76-1/60-7/3600</f>
+        <v>-76.018611111111113</v>
+      </c>
+      <c r="O230">
+        <v>28</v>
+      </c>
+      <c r="Q230" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="231" spans="1:17" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A231" s="4">
         <v>260</v>
       </c>
@@ -13174,13 +13293,16 @@
         <v>-110.963855204659</v>
       </c>
       <c r="O231">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P231" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="232" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q231" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="232" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A232" s="4">
         <v>261</v>
       </c>
@@ -13225,10 +13347,13 @@
         <v>21</v>
       </c>
       <c r="P232" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="233" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q232" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="233" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A233" s="4">
         <v>262</v>
       </c>
@@ -13273,10 +13398,13 @@
         <v>6</v>
       </c>
       <c r="P233" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="234" spans="1:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q233" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="234" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A234" s="4">
         <v>263</v>
       </c>
@@ -13323,7 +13451,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="235" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A235" s="4">
         <v>264</v>
       </c>
@@ -13365,10 +13493,13 @@
         <v>-105.915166208657</v>
       </c>
       <c r="P235" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="236" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q235" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="236" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A236" s="4">
         <v>265</v>
       </c>
@@ -13410,10 +13541,13 @@
         <v>-105.915166208657</v>
       </c>
       <c r="P236" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="237" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q236" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="237" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A237" s="4">
         <v>266</v>
       </c>
@@ -13458,10 +13592,13 @@
         <v>6</v>
       </c>
       <c r="P237" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="238" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q237" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="238" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A238" s="4">
         <v>267</v>
       </c>
@@ -13508,7 +13645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="239" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A239" s="4">
         <v>268</v>
       </c>
@@ -13554,11 +13691,11 @@
       <c r="O239">
         <v>8</v>
       </c>
-      <c r="P239" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q239" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="240" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A240" s="4">
         <v>269</v>
       </c>
@@ -13604,11 +13741,11 @@
       <c r="O240">
         <v>1</v>
       </c>
-      <c r="P240" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="241" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q240" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="241" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A241" s="4">
         <v>270</v>
       </c>
@@ -13655,11 +13792,11 @@
         <f>1981-1957</f>
         <v>24</v>
       </c>
-      <c r="P241" s="19" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="242" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q241" s="15" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="242" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A242" s="4">
         <v>271</v>
       </c>
@@ -13705,11 +13842,11 @@
       <c r="O242">
         <v>20</v>
       </c>
-      <c r="P242" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="243" spans="1:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="Q242" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="243" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A243" s="4">
         <v>272</v>
       </c>
@@ -13753,11 +13890,11 @@
       <c r="O243">
         <v>17</v>
       </c>
-      <c r="P243" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="244" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="Q243" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="244" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A244" s="4">
         <v>273</v>
       </c>
@@ -13802,10 +13939,13 @@
         <v>8</v>
       </c>
       <c r="P244" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="245" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q244" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="245" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A245" s="4">
         <v>274</v>
       </c>
@@ -13850,7 +13990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A246" s="4">
         <v>275</v>
       </c>
@@ -13895,10 +14035,13 @@
         <v>10</v>
       </c>
       <c r="P246" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="247" spans="1:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q246" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="247" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A247" s="4">
         <v>276</v>
       </c>
@@ -13943,10 +14086,13 @@
         <v>10</v>
       </c>
       <c r="P247" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="248" spans="1:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q247" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="248" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A248" s="4">
         <v>277</v>
       </c>
@@ -13991,10 +14137,13 @@
         <v>10</v>
       </c>
       <c r="P248" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="249" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q248" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="249" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A249" s="4">
         <v>278</v>
       </c>
@@ -14039,11 +14188,11 @@
       <c r="O249">
         <v>8</v>
       </c>
-      <c r="P249" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q249" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="250" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A250" s="4">
         <v>279</v>
       </c>
@@ -14088,10 +14237,13 @@
         <v>9</v>
       </c>
       <c r="P250" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q250" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="251" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A251" s="4">
         <v>280</v>
       </c>
@@ -14136,10 +14288,13 @@
         <v>7</v>
       </c>
       <c r="P251" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="252" spans="1:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="Q251" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="252" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A252" s="4">
         <v>281</v>
       </c>
@@ -14186,7 +14341,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="253" spans="1:16" ht="41.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:17" ht="41.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A253" s="6">
         <v>282</v>
       </c>
@@ -14247,7 +14402,7 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="P241" r:id="rId1" display="https://www2.ffpri.go.jp/labs/fwdb/sites/takaragawaE.htm reference should be Bosch, J.M., Hewlett, J.D., 1982. A review of catchment experiments to determine the effect of vegetation changes on water yield and evapotranspiration. Journal of Hydrology, 55: 3-23. " xr:uid="{5309022A-E206-41E7-A5C0-F8D3DD4A0F00}"/>
+    <hyperlink ref="Q241" r:id="rId1" display="https://www2.ffpri.go.jp/labs/fwdb/sites/takaragawaE.htm reference should be Bosch, J.M., Hewlett, J.D., 1982. A review of catchment experiments to determine the effect of vegetation changes on water yield and evapotranspiration. Journal of Hydrology, 55: 3-23. " xr:uid="{5309022A-E206-41E7-A5C0-F8D3DD4A0F00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
@@ -14258,8 +14413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD75620-6F76-4BA6-A94E-CE93109D006F}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18:M18"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14268,54 +14423,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
       <c r="L2" t="s">
         <v>527</v>
       </c>
@@ -15088,7 +15243,7 @@
         <v>10</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
coordinate update and renumbered new data
</commit_message>
<xml_diff>
--- a/data/TablesZhangetal2017_WV.xlsx
+++ b/data/TablesZhangetal2017_WV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6963F5-A3CB-49DC-B8E5-659BB61DA4E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424A4A01-DE76-4C79-A381-39F283691BF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12624" activeTab="1" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
+    <workbookView xWindow="22690" yWindow="3630" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
   </bookViews>
   <sheets>
     <sheet name="Zhang et al. (2017) &gt;1000km2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="615">
   <si>
     <t>Watershed #</t>
   </si>
@@ -1840,9 +1840,6 @@
     <t>coordinates guessed from google maps</t>
   </si>
   <si>
-    <t>The tree felling is actually incremental in time, so not really a single observation</t>
-  </si>
-  <si>
     <t>time period guessed from Fig 5 in Beck et al.</t>
   </si>
   <si>
@@ -1855,9 +1852,6 @@
     <t>time period to the first change point in Webb and Jarrett (2013)</t>
   </si>
   <si>
-    <t>There is no Yerrami S in Zhou et al.</t>
-  </si>
-  <si>
     <t>Bosboukloof</t>
   </si>
   <si>
@@ -1910,6 +1904,30 @@
   </si>
   <si>
     <t>Location from https://waterdata.usgs.gov/ Not in Brown et al. (2005), but in Bosch and Hewlett (1982). Original reference is Schneider and Ayer (1961), U.S. Geol. Surv., Water-Supply Pap. 1602.</t>
+  </si>
+  <si>
+    <t>The tree felling is actually incremental in time, so not really a single observation. In addition, there are no clear individual coordinates for the subcatchments in Plynlimon. We probably need to download the shapefiles.</t>
+  </si>
+  <si>
+    <t>coordinates from USGS</t>
+  </si>
+  <si>
+    <t>usgs coordinates</t>
+  </si>
+  <si>
+    <t>coordinates usgs</t>
+  </si>
+  <si>
+    <t>Another catchment in Bart and Hope that was for some reason not added originally. Coordinates from usgs</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>There is no Yerrami S in Zhou et al. This is originally from Ruprecht and Schofield (1989), but they are citing a WA water resources report</t>
+  </si>
+  <si>
+    <t>coordinates from usgs</t>
   </si>
 </sst>
 </file>
@@ -4582,14 +4600,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C628113C-78B0-4B5D-8B46-887DA17257C6}">
   <dimension ref="A1:Q253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="B231" sqref="B231"/>
+    <sheetView tabSelected="1" topLeftCell="C220" workbookViewId="0">
+      <selection activeCell="Q226" sqref="Q226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -5574,7 +5591,7 @@
         <v>1</v>
       </c>
       <c r="Q26" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -5756,6 +5773,20 @@
         <v>174</v>
       </c>
       <c r="L31" s="11"/>
+      <c r="M31">
+        <f>36+24/60+8/3600</f>
+        <v>36.402222222222221</v>
+      </c>
+      <c r="N31">
+        <f>-120-25/60-57/3600</f>
+        <v>-120.4325</v>
+      </c>
+      <c r="O31">
+        <v>5</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>609</v>
+      </c>
     </row>
     <row r="32" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
@@ -5948,7 +5979,7 @@
         <v>26</v>
       </c>
       <c r="Q36" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -6213,7 +6244,7 @@
         <v>-75.392777777777781</v>
       </c>
       <c r="Q43" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
@@ -8012,7 +8043,7 @@
         <v>30</v>
       </c>
       <c r="Q92" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -8060,7 +8091,7 @@
         <v>30</v>
       </c>
       <c r="Q93" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -8108,7 +8139,7 @@
         <v>30</v>
       </c>
       <c r="Q94" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
@@ -8228,7 +8259,7 @@
         <v>30</v>
       </c>
       <c r="Q97" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="98" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -8276,7 +8307,7 @@
         <v>30</v>
       </c>
       <c r="Q98" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="99" spans="1:17" ht="61.2" x14ac:dyDescent="0.3">
@@ -8321,7 +8352,7 @@
         <v>-105.92363805782</v>
       </c>
       <c r="Q99" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="100" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -9821,6 +9852,17 @@
         <v>174</v>
       </c>
       <c r="L140" s="4"/>
+      <c r="M140">
+        <f>35+14/60+8/3600</f>
+        <v>35.235555555555557</v>
+      </c>
+      <c r="N140">
+        <f>-120-28/60-17/3600</f>
+        <v>-120.4713888888889</v>
+      </c>
+      <c r="O140">
+        <v>5</v>
+      </c>
     </row>
     <row r="141" spans="1:17" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="6">
@@ -10599,7 +10641,7 @@
         <v>1</v>
       </c>
       <c r="Q161" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="162" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
@@ -10683,7 +10725,7 @@
         <v>6</v>
       </c>
       <c r="Q163" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="164" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -10731,7 +10773,7 @@
         <v>3</v>
       </c>
       <c r="Q164" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="165" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -11768,7 +11810,7 @@
       </c>
       <c r="L192" s="4"/>
     </row>
-    <row r="193" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A193" s="4">
         <v>252</v>
       </c>
@@ -11804,7 +11846,7 @@
       </c>
       <c r="L193" s="4"/>
     </row>
-    <row r="194" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A194" s="4">
         <v>253</v>
       </c>
@@ -11840,7 +11882,7 @@
       </c>
       <c r="L194" s="4"/>
     </row>
-    <row r="195" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A195" s="4">
         <v>254</v>
       </c>
@@ -11876,7 +11918,7 @@
       </c>
       <c r="L195" s="4"/>
     </row>
-    <row r="196" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A196" s="4">
         <v>255</v>
       </c>
@@ -11912,7 +11954,7 @@
       </c>
       <c r="L196" s="4"/>
     </row>
-    <row r="197" spans="1:12" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:17" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A197" s="6">
         <v>256</v>
       </c>
@@ -11947,8 +11989,22 @@
         <v>174</v>
       </c>
       <c r="L197" s="11"/>
-    </row>
-    <row r="198" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="M197">
+        <f>34+24/60+48/3600</f>
+        <v>34.413333333333334</v>
+      </c>
+      <c r="N197">
+        <f>-119-4/60-23/3600</f>
+        <v>-119.07305555555556</v>
+      </c>
+      <c r="O197">
+        <v>5</v>
+      </c>
+      <c r="Q197" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="198" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A198" s="4">
         <v>283</v>
       </c>
@@ -11984,7 +12040,7 @@
       </c>
       <c r="L198" s="4"/>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A199" s="4">
         <v>284</v>
       </c>
@@ -12020,7 +12076,7 @@
       </c>
       <c r="L199" s="4"/>
     </row>
-    <row r="200" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A200" s="4">
         <v>285</v>
       </c>
@@ -12056,7 +12112,7 @@
       </c>
       <c r="L200" s="4"/>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A201" s="4">
         <v>286</v>
       </c>
@@ -12092,7 +12148,7 @@
       </c>
       <c r="L201" s="4"/>
     </row>
-    <row r="202" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A202" s="4">
         <v>287</v>
       </c>
@@ -12128,7 +12184,7 @@
       </c>
       <c r="L202" s="4"/>
     </row>
-    <row r="203" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A203" s="4">
         <v>288</v>
       </c>
@@ -12164,7 +12220,7 @@
       </c>
       <c r="L203" s="4"/>
     </row>
-    <row r="204" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A204" s="4">
         <v>289</v>
       </c>
@@ -12200,7 +12256,7 @@
       </c>
       <c r="L204" s="4"/>
     </row>
-    <row r="205" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A205" s="4">
         <v>290</v>
       </c>
@@ -12236,7 +12292,7 @@
       </c>
       <c r="L205" s="4"/>
     </row>
-    <row r="206" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A206" s="4">
         <v>291</v>
       </c>
@@ -12272,7 +12328,7 @@
       </c>
       <c r="L206" s="4"/>
     </row>
-    <row r="207" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A207" s="4">
         <v>292</v>
       </c>
@@ -12308,7 +12364,7 @@
       </c>
       <c r="L207" s="4"/>
     </row>
-    <row r="208" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A208" s="4">
         <v>293</v>
       </c>
@@ -12692,10 +12748,10 @@
         <v>5</v>
       </c>
       <c r="P217" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q217" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="218" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
@@ -12740,10 +12796,10 @@
         <v>-110.963855204659</v>
       </c>
       <c r="P218" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q218" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="219" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
@@ -12791,10 +12847,10 @@
         <v>11</v>
       </c>
       <c r="P219" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q219" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="220" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
@@ -12842,10 +12898,10 @@
         <v>13</v>
       </c>
       <c r="P220" t="s">
+        <v>596</v>
+      </c>
+      <c r="Q220" t="s">
         <v>598</v>
-      </c>
-      <c r="Q220" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="221" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
@@ -12893,10 +12949,10 @@
         <v>11</v>
       </c>
       <c r="P221" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q221" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="222" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -13042,6 +13098,20 @@
         <v>523</v>
       </c>
       <c r="L225" s="4"/>
+      <c r="M225">
+        <f>43+57/60+17.45/3600</f>
+        <v>43.954847222222227</v>
+      </c>
+      <c r="N225">
+        <f>-71-43/60-22.21/3600</f>
+        <v>-71.722836111111107</v>
+      </c>
+      <c r="O225">
+        <v>25</v>
+      </c>
+      <c r="Q225" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="226" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A226" s="4">
@@ -13125,8 +13195,20 @@
         <v>345</v>
       </c>
       <c r="L227" s="11"/>
+      <c r="M227">
+        <v>-34.1738338289274</v>
+      </c>
+      <c r="N227">
+        <v>116.379359835201</v>
+      </c>
+      <c r="O227">
+        <v>5</v>
+      </c>
+      <c r="P227" t="s">
+        <v>596</v>
+      </c>
       <c r="Q227" t="s">
-        <v>590</v>
+        <v>613</v>
       </c>
     </row>
     <row r="228" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -13164,6 +13246,20 @@
         <v>174</v>
       </c>
       <c r="L228" s="11"/>
+      <c r="M228">
+        <f>34+34/60+10/3600</f>
+        <v>34.56944444444445</v>
+      </c>
+      <c r="N228">
+        <f>-119-15/60-23/3600</f>
+        <v>-119.25638888888889</v>
+      </c>
+      <c r="O228">
+        <v>5</v>
+      </c>
+      <c r="Q228" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="229" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A229" s="4">
@@ -13200,6 +13296,18 @@
         <v>299</v>
       </c>
       <c r="L229" s="4"/>
+      <c r="M229">
+        <v>52.472088267260901</v>
+      </c>
+      <c r="N229">
+        <v>-3.71674779431117</v>
+      </c>
+      <c r="O229">
+        <v>17</v>
+      </c>
+      <c r="P229" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="230" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A230" s="4">
@@ -13248,7 +13356,7 @@
         <v>28</v>
       </c>
       <c r="Q230" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="231" spans="1:17" ht="61.2" x14ac:dyDescent="0.3">
@@ -13296,10 +13404,10 @@
         <v>1</v>
       </c>
       <c r="P231" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q231" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="232" spans="1:17" ht="30.6" x14ac:dyDescent="0.3">
@@ -13347,7 +13455,7 @@
         <v>21</v>
       </c>
       <c r="P232" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q232" t="s">
         <v>584</v>
@@ -13398,7 +13506,7 @@
         <v>6</v>
       </c>
       <c r="P233" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q233" t="s">
         <v>584</v>
@@ -13493,10 +13601,10 @@
         <v>-105.915166208657</v>
       </c>
       <c r="P235" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q235" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="236" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -13541,7 +13649,7 @@
         <v>-105.915166208657</v>
       </c>
       <c r="P236" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q236" t="s">
         <v>584</v>
@@ -13592,7 +13700,7 @@
         <v>6</v>
       </c>
       <c r="P237" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q237" t="s">
         <v>584</v>
@@ -13692,7 +13800,7 @@
         <v>8</v>
       </c>
       <c r="Q239" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="240" spans="1:17" x14ac:dyDescent="0.3">
@@ -13742,7 +13850,7 @@
         <v>1</v>
       </c>
       <c r="Q240" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="241" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -13793,7 +13901,7 @@
         <v>24</v>
       </c>
       <c r="Q241" s="15" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="242" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -13843,7 +13951,7 @@
         <v>20</v>
       </c>
       <c r="Q242" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="243" spans="1:17" ht="40.799999999999997" x14ac:dyDescent="0.3">
@@ -13890,8 +13998,11 @@
       <c r="O243">
         <v>17</v>
       </c>
+      <c r="P243" t="s">
+        <v>596</v>
+      </c>
       <c r="Q243" t="s">
-        <v>585</v>
+        <v>607</v>
       </c>
     </row>
     <row r="244" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -13939,7 +14050,7 @@
         <v>8</v>
       </c>
       <c r="P244" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q244" t="s">
         <v>584</v>
@@ -14035,7 +14146,7 @@
         <v>10</v>
       </c>
       <c r="P246" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q246" t="s">
         <v>584</v>
@@ -14086,7 +14197,7 @@
         <v>10</v>
       </c>
       <c r="P247" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q247" t="s">
         <v>584</v>
@@ -14137,7 +14248,7 @@
         <v>10</v>
       </c>
       <c r="P248" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q248" t="s">
         <v>584</v>
@@ -14237,7 +14348,7 @@
         <v>9</v>
       </c>
       <c r="P250" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q250" t="s">
         <v>581</v>
@@ -14288,7 +14399,7 @@
         <v>7</v>
       </c>
       <c r="P251" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Q251" t="s">
         <v>581</v>
@@ -14411,15 +14522,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD75620-6F76-4BA6-A94E-CE93109D006F}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -14489,7 +14601,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>283</v>
+        <v>313</v>
       </c>
       <c r="B3" t="s">
         <v>529</v>
@@ -14536,7 +14648,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>284</v>
+        <v>314</v>
       </c>
       <c r="B4" t="s">
         <v>531</v>
@@ -14583,7 +14695,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>285</v>
+        <v>315</v>
       </c>
       <c r="B5" t="s">
         <v>533</v>
@@ -14630,7 +14742,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>286</v>
+        <v>316</v>
       </c>
       <c r="B6" t="s">
         <v>534</v>
@@ -14677,7 +14789,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>287</v>
+        <v>317</v>
       </c>
       <c r="B7" t="s">
         <v>535</v>
@@ -14724,7 +14836,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>288</v>
+        <v>318</v>
       </c>
       <c r="B8" t="s">
         <v>536</v>
@@ -14771,7 +14883,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>289</v>
+        <v>319</v>
       </c>
       <c r="B9" t="s">
         <v>537</v>
@@ -14818,7 +14930,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>290</v>
+        <v>320</v>
       </c>
       <c r="B10" t="s">
         <v>538</v>
@@ -14865,7 +14977,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>291</v>
+        <v>321</v>
       </c>
       <c r="B11" t="s">
         <v>539</v>
@@ -14912,7 +15024,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>292</v>
+        <v>322</v>
       </c>
       <c r="B12" t="s">
         <v>540</v>
@@ -14959,7 +15071,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>293</v>
+        <v>323</v>
       </c>
       <c r="B13" t="s">
         <v>541</v>
@@ -15005,8 +15117,8 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
-        <v>294</v>
+      <c r="A14">
+        <v>324</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>432</v>
@@ -15059,7 +15171,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>295</v>
+        <v>325</v>
       </c>
       <c r="B15" t="s">
         <v>542</v>
@@ -15106,7 +15218,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>296</v>
+        <v>326</v>
       </c>
       <c r="B16" t="s">
         <v>543</v>
@@ -15153,7 +15265,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>297</v>
+        <v>327</v>
       </c>
       <c r="B17" t="s">
         <v>544</v>
@@ -15199,8 +15311,8 @@
       </c>
     </row>
     <row r="18" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12">
-        <v>298</v>
+      <c r="A18">
+        <v>328</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>546</v>
@@ -15248,7 +15360,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>299</v>
+        <v>329</v>
       </c>
       <c r="B19" t="s">
         <v>547</v>
@@ -15298,7 +15410,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="B20" t="s">
         <v>563</v>
@@ -15348,7 +15460,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>301</v>
+        <v>331</v>
       </c>
       <c r="B21" t="s">
         <v>552</v>
@@ -15398,7 +15510,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>304</v>
+        <v>332</v>
       </c>
       <c r="B22" t="s">
         <v>561</v>
@@ -15448,7 +15560,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>305</v>
+        <v>333</v>
       </c>
       <c r="B23" t="s">
         <v>566</v>
@@ -15495,7 +15607,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>306</v>
+        <v>334</v>
       </c>
       <c r="B24" t="s">
         <v>567</v>
@@ -15548,7 +15660,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>307</v>
+        <v>335</v>
       </c>
       <c r="B25" t="s">
         <v>570</v>
@@ -15598,7 +15710,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>308</v>
+        <v>336</v>
       </c>
       <c r="B26" t="s">
         <v>573</v>
@@ -15645,6 +15757,55 @@
       </c>
       <c r="Q26" t="s">
         <v>575</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>337</v>
+      </c>
+      <c r="B27" t="s">
+        <v>612</v>
+      </c>
+      <c r="C27">
+        <v>104</v>
+      </c>
+      <c r="D27">
+        <v>680</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="6">
+        <v>-32</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="L27">
+        <f>35+53/60+48/3600</f>
+        <v>35.896666666666668</v>
+      </c>
+      <c r="M27">
+        <f>-121-5/60-14/3600</f>
+        <v>-121.08722222222222</v>
+      </c>
+      <c r="O27">
+        <v>5</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>